<commit_message>
update vaccine averted deaths
</commit_message>
<xml_diff>
--- a/data/Vaccine profile for IHME burden.xlsx
+++ b/data/Vaccine profile for IHME burden.xlsx
@@ -5,21 +5,23 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ivionline-my.sharepoint.com/personal/chaelin_kim_ivi_int/Documents/Documents/GitHub/vaccine_amr/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaelin.kim\OneDrive - International Vaccine Institute\Documents\GitHub\vaccine_amr\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{51B251E8-8EFC-40BD-9661-7D42E9522303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F914DB2A-07BA-4057-B0A4-EED720A6CCC7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49439271-20EA-4986-AD43-7915C30B9E96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="2" xr2:uid="{E3505429-E9FF-3944-B32E-F1BA65C67D7B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="2" activeTab="3" xr2:uid="{E3505429-E9FF-3944-B32E-F1BA65C67D7B}"/>
   </bookViews>
   <sheets>
     <sheet name="SIGs" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="Vaccine profile assumptions" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="7" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Sheet3!$A$1:$G$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SIGs!$A$1:$K$43</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Vaccine profile assumptions'!$A$1:$K$26</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Vaccine profile assumptions'!$A$1:$L$26</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -73,8 +75,42 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Chaelin Kim</author>
+  </authors>
+  <commentList>
+    <comment ref="B5" authorId="0" shapeId="0" xr:uid="{CB536B3A-0091-416A-86ED-EC21FCE09D12}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Chaelin Kim:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+65-80</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="346">
   <si>
     <t>Who</t>
   </si>
@@ -2456,10 +2492,7 @@
     <t>BSI, LRI and thorax infections</t>
   </si>
   <si>
-    <t>LRI and throx infections</t>
-  </si>
-  <si>
-    <t>All, but 50% for LRI and throx infections</t>
+    <t>All (50% for LRI and throx infections)</t>
   </si>
 </sst>
 </file>
@@ -4644,9 +4677,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -4700,7 +4733,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="156" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" ht="156" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>252</v>
       </c>
@@ -4776,7 +4809,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="109.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>260</v>
       </c>
@@ -4814,7 +4847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="109.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>263</v>
       </c>
@@ -4890,7 +4923,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="62.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A7" s="19" t="s">
         <v>271</v>
       </c>
@@ -5042,7 +5075,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="171.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
         <v>286</v>
       </c>
@@ -5118,7 +5151,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="46.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A13" s="19" t="s">
         <v>294</v>
       </c>
@@ -5156,7 +5189,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="96.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" ht="96.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="46" t="s">
         <v>332</v>
       </c>
@@ -5232,7 +5265,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:12" s="43" customFormat="1" ht="140.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" s="43" customFormat="1" ht="140.4" x14ac:dyDescent="0.3">
       <c r="A16" s="42" t="s">
         <v>300</v>
       </c>
@@ -5308,7 +5341,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:12" ht="109.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>306</v>
       </c>
@@ -5384,7 +5417,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:12" ht="202.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="202.8" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>317</v>
       </c>
@@ -5422,7 +5455,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="109.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="19" t="s">
         <v>321</v>
       </c>
@@ -5448,7 +5481,7 @@
         <v>76</v>
       </c>
       <c r="I21" s="36" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="J21" s="36" t="s">
         <v>339</v>
@@ -5460,7 +5493,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="22" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="109.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>321</v>
       </c>
@@ -5498,7 +5531,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="23" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="109.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="19" t="s">
         <v>321</v>
       </c>
@@ -5562,7 +5595,7 @@
         <v>225</v>
       </c>
       <c r="I24" s="36" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="J24" s="36" t="s">
         <v>339</v>
@@ -5574,7 +5607,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="109.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="19" t="s">
         <v>327</v>
       </c>
@@ -5612,7 +5645,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="109.2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="109.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>327</v>
       </c>
@@ -5651,10 +5684,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K26" xr:uid="{6A9E86CB-7D0A-7349-B091-299D92D6946C}">
-    <filterColumn colId="9">
+  <autoFilter ref="A1:L26" xr:uid="{6A9E86CB-7D0A-7349-B091-299D92D6946C}">
+    <filterColumn colId="11">
       <filters>
-        <filter val="4 week (effective at 6 week)"/>
+        <filter val="Yes"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -5664,22 +5697,400 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79A4DC60-5142-4373-A463-244441A1357F}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20.19921875" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" customWidth="1"/>
+    <col min="3" max="3" width="14.3984375" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" customWidth="1"/>
+    <col min="5" max="6" width="15.19921875" style="19" customWidth="1"/>
+    <col min="7" max="7" width="24.69921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>248</v>
+      </c>
+      <c r="E1" s="35" t="s">
+        <v>249</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>250</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="36" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>70</v>
+      </c>
+      <c r="C2">
+        <v>70</v>
+      </c>
+      <c r="D2" s="34">
+        <v>5</v>
+      </c>
+      <c r="E2" s="40" t="s">
+        <v>256</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3">
+        <v>70</v>
+      </c>
+      <c r="C3">
+        <v>70</v>
+      </c>
+      <c r="D3" s="34">
+        <v>5</v>
+      </c>
+      <c r="E3" s="39" t="s">
+        <v>257</v>
+      </c>
+      <c r="F3" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="G3" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4">
+        <v>70</v>
+      </c>
+      <c r="C4">
+        <v>70</v>
+      </c>
+      <c r="D4" s="34">
+        <v>2</v>
+      </c>
+      <c r="E4" s="40" t="s">
+        <v>275</v>
+      </c>
+      <c r="F4" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="G4" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5">
+        <v>72.5</v>
+      </c>
+      <c r="C5">
+        <v>90</v>
+      </c>
+      <c r="D5" s="34">
+        <v>5</v>
+      </c>
+      <c r="E5" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F5" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="36" t="s">
+        <v>281</v>
+      </c>
+      <c r="B6">
+        <v>90</v>
+      </c>
+      <c r="C6">
+        <v>90</v>
+      </c>
+      <c r="D6" s="34">
+        <v>5</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F6" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="36" t="s">
+        <v>284</v>
+      </c>
+      <c r="B7">
+        <v>70</v>
+      </c>
+      <c r="C7">
+        <v>70</v>
+      </c>
+      <c r="D7" s="34">
+        <v>5</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="36" t="s">
+        <v>291</v>
+      </c>
+      <c r="B8">
+        <v>80</v>
+      </c>
+      <c r="C8">
+        <v>70</v>
+      </c>
+      <c r="D8" s="34">
+        <v>10</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>338</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="47" t="s">
+        <v>335</v>
+      </c>
+      <c r="B9" s="47">
+        <v>70</v>
+      </c>
+      <c r="C9" s="47">
+        <v>70</v>
+      </c>
+      <c r="D9" s="47">
+        <v>10</v>
+      </c>
+      <c r="E9" s="46" t="s">
+        <v>341</v>
+      </c>
+      <c r="F9" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="G9" s="46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A10" s="36" t="s">
+        <v>298</v>
+      </c>
+      <c r="B10">
+        <v>80</v>
+      </c>
+      <c r="C10">
+        <v>70</v>
+      </c>
+      <c r="D10" s="34">
+        <v>5</v>
+      </c>
+      <c r="E10" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F10" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="42" t="s">
+        <v>159</v>
+      </c>
+      <c r="B11" s="43">
+        <v>70</v>
+      </c>
+      <c r="C11" s="43">
+        <v>70</v>
+      </c>
+      <c r="D11" s="44">
+        <v>1</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>344</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>338</v>
+      </c>
+      <c r="G11" s="42" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A12" s="36" t="s">
+        <v>304</v>
+      </c>
+      <c r="B12">
+        <v>70</v>
+      </c>
+      <c r="C12">
+        <v>90</v>
+      </c>
+      <c r="D12" s="34">
+        <v>5</v>
+      </c>
+      <c r="E12" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="G12" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="31.2" x14ac:dyDescent="0.3">
+      <c r="A13" s="36" t="s">
+        <v>307</v>
+      </c>
+      <c r="B13">
+        <v>85</v>
+      </c>
+      <c r="C13">
+        <v>70</v>
+      </c>
+      <c r="D13" s="34">
+        <v>20</v>
+      </c>
+      <c r="E13" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F13" s="36" t="s">
+        <v>310</v>
+      </c>
+      <c r="G13" s="19" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="62.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="36" t="s">
+        <v>314</v>
+      </c>
+      <c r="B14">
+        <v>60</v>
+      </c>
+      <c r="C14">
+        <v>70</v>
+      </c>
+      <c r="D14" s="34">
+        <v>5</v>
+      </c>
+      <c r="E14" s="36" t="s">
+        <v>343</v>
+      </c>
+      <c r="F14" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="36" t="s">
+        <v>318</v>
+      </c>
+      <c r="B15">
+        <v>60</v>
+      </c>
+      <c r="C15">
+        <v>70</v>
+      </c>
+      <c r="D15" s="34">
+        <v>2</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>257</v>
+      </c>
+      <c r="F15" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="36" t="s">
+        <v>323</v>
+      </c>
+      <c r="B16">
+        <v>70</v>
+      </c>
+      <c r="C16">
+        <v>90</v>
+      </c>
+      <c r="D16" s="34">
+        <v>2</v>
+      </c>
+      <c r="E16" s="36" t="s">
+        <v>345</v>
+      </c>
+      <c r="F16" s="36" t="s">
+        <v>339</v>
+      </c>
+      <c r="G16" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G16" xr:uid="{79A4DC60-5142-4373-A463-244441A1357F}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000FED123832FD0488CFCE1AA10E1DCD4" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="41a705e68a8aeb9b58d52370ca01447e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="a45b7c79-9df6-4e54-8c6e-a05b6926a077" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ba608db981251bffcca843424efdcbba" ns3:_="">
     <xsd:import namespace="a45b7c79-9df6-4e54-8c6e-a05b6926a077"/>
@@ -5863,24 +6274,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{949C4874-4D5A-4FE9-8546-A8417F100372}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2737EBF5-6B84-4C51-A2EC-BF7D423E712E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F71E18D2-388C-40B5-9487-62F8D977B285}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5896,4 +6305,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2737EBF5-6B84-4C51-A2EC-BF7D423E712E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{949C4874-4D5A-4FE9-8546-A8417F100372}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>